<commit_message>
Modification du fichier .xlsx
</commit_message>
<xml_diff>
--- a/DEM_COM.xlsx
+++ b/DEM_COM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KelennTech\Applications\smartVdg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarik\Applications\smartVdgRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -131,11 +131,11 @@
     <t xml:space="preserve">#CMD_[num_ordre] kpm stop_job </t>
   </si>
   <si>
-    <t>#CPT_[num_ordre] BOX CHANGE [nomJob] [num_theo] [num_reel]</t>
-  </si>
-  <si>
     <t xml:space="preserve">au finale KMP aura un stop job c'est la seule condition qui permet de créer
 le dernier contenant s'il n'atteint pas le nombre maximum de pli / Ke7 </t>
+  </si>
+  <si>
+    <t>#CPT_[num_ordre] BOX CHANGE [nomJob] [num_theo] [num_reel] [FST]</t>
   </si>
 </sst>
 </file>
@@ -220,18 +220,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,7 +550,7 @@
   <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,26 +566,26 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
@@ -593,7 +593,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -601,10 +601,10 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
@@ -617,10 +617,10 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="6" t="s">
         <v>28</v>
       </c>
@@ -633,10 +633,10 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
@@ -649,10 +649,10 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="2" t="s">
         <v>31</v>
       </c>
@@ -665,10 +665,10 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
@@ -684,12 +684,12 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>7</v>
@@ -703,10 +703,10 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
@@ -719,10 +719,10 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
@@ -735,10 +735,10 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
@@ -751,10 +751,10 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
@@ -762,18 +762,18 @@
         <v>13</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="13" t="s">
-        <v>35</v>
+      <c r="G13" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
@@ -786,10 +786,10 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="5" t="s">
         <v>19</v>
       </c>
@@ -822,12 +822,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -836,6 +830,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Modification du fichier .xlsx"
This reverts commit a92a9057572d6d756591d9f6f5d72038c3fa03c9.
</commit_message>
<xml_diff>
--- a/DEM_COM.xlsx
+++ b/DEM_COM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarik\Applications\smartVdgRepo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KelennTech\Applications\smartVdg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -131,11 +131,11 @@
     <t xml:space="preserve">#CMD_[num_ordre] kpm stop_job </t>
   </si>
   <si>
+    <t>#CPT_[num_ordre] BOX CHANGE [nomJob] [num_theo] [num_reel]</t>
+  </si>
+  <si>
     <t xml:space="preserve">au finale KMP aura un stop job c'est la seule condition qui permet de créer
 le dernier contenant s'il n'atteint pas le nombre maximum de pli / Ke7 </t>
-  </si>
-  <si>
-    <t>#CPT_[num_ordre] BOX CHANGE [nomJob] [num_theo] [num_reel] [FST]</t>
   </si>
 </sst>
 </file>
@@ -220,18 +220,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,7 +550,7 @@
   <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,26 +566,26 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
@@ -593,7 +593,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -601,10 +601,10 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
@@ -617,10 +617,10 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="6" t="s">
         <v>28</v>
       </c>
@@ -633,10 +633,10 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
@@ -649,10 +649,10 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="2" t="s">
         <v>31</v>
       </c>
@@ -665,10 +665,10 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
@@ -684,12 +684,12 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>7</v>
@@ -703,10 +703,10 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
@@ -719,10 +719,10 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
@@ -735,10 +735,10 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
@@ -751,10 +751,10 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
@@ -762,18 +762,18 @@
         <v>13</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="10" t="s">
-        <v>34</v>
+      <c r="G13" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
@@ -786,10 +786,10 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="13"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="5" t="s">
         <v>19</v>
       </c>
@@ -822,6 +822,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -830,12 +836,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>